<commit_message>
Normalize sports and fix templates
</commit_message>
<xml_diff>
--- a/sports_templates.xlsx
+++ b/sports_templates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alphonsusteow/Documents/alph_projects/SportSG/CodeProjects/major_games_reporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5ABDA9-ADD3-DD45-B185-47720AB87238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08683133-9DC8-744F-8633-8FCE3B14662E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Templates" sheetId="1" r:id="rId1"/>
@@ -56,12 +56,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All Templates'!$A$1:$H$199</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3495" uniqueCount="1318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3495" uniqueCount="1319">
   <si>
     <t>sport</t>
   </si>
@@ -5745,6 +5758,9 @@
   </si>
   <si>
     <t>Sailing</t>
+  </si>
+  <si>
+    <t>Ju-Jitsu</t>
   </si>
 </sst>
 </file>
@@ -6117,9 +6133,9 @@
   <dimension ref="A1:H199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8344,7 +8360,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>386</v>
       </c>
@@ -8370,7 +8386,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>386</v>
       </c>
@@ -12904,9 +12920,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -12950,7 +12971,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>587</v>
+        <v>891</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -12958,7 +12979,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>328</v>
+        <v>888</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -12974,7 +12995,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>451</v>
+        <v>890</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -12990,7 +13011,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>692</v>
+        <v>892</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -13006,7 +13027,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>862</v>
+        <v>894</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -13022,7 +13043,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>885</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -13038,7 +13059,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>886</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -13070,7 +13091,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>751</v>
+        <v>1318</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -13110,7 +13131,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>409</v>
+        <v>1317</v>
       </c>
       <c r="B26">
         <v>5</v>
@@ -13142,7 +13163,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>206</v>
+        <v>887</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -13198,7 +13219,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>715</v>
+        <v>893</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -15145,7 +15166,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -17277,9 +17300,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="32.1640625" customWidth="1"/>
+    <col min="6" max="6" width="48.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -18031,9 +18061,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="165.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>